<commit_message>
update calculator tool exports to include costs per indicator
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575CC4E6-4F93-8A45-BB7A-BD10F698B1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC96A000-EF53-C641-AA38-A147322CADAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="452">
   <si>
     <t>Text</t>
   </si>
@@ -480,9 +480,6 @@
     <t>This data dictionary is intended to document the dataset(s) accessible at https://github.com/cghss/IHR-costing</t>
   </si>
   <si>
-    <t>The data dictionary was last updated on July 7, 2023</t>
-  </si>
-  <si>
     <t>If you have any questions, please reach out to sde31@georgetown.edu</t>
   </si>
   <si>
@@ -940,12 +937,6 @@
   </si>
   <si>
     <t>The category of the cost (personnel, operating, or transport) based on the categorizations defined by Sloan et al in Sloan ML, Gleason BL, Squire JS, Koroma FF, Sogbeh SA, Park MJ. Cost Analysis of Health Facility Electronic Integrated Disease Surveillance and Response in One District in Sierra Leone. Health Security. 2020 Jan 1;18(S1):S-64-S-71.</t>
-  </si>
-  <si>
-    <t>The category of the cost based on the cost categories defined by GHSS. Please see methods documentation for more detailed definitions</t>
-  </si>
-  <si>
-    <t>The subcategory of the cost based on the cost categories defined by GHSS. Please see methods documentation for more detailed definitions</t>
   </si>
   <si>
     <t>The name of the default unit cost</t>
@@ -1293,6 +1284,163 @@
   </si>
   <si>
     <t>JEE 3.0 specifies that "The recommended density of doctors, nurses and midwives per 1000 population for operational routine services is 4.45 plus 30% surge capacity"</t>
+  </si>
+  <si>
+    <t>The category of the cost based on the cost categories defined by GHSS. Please see methods documentation and definitions tab for more detailed definitions</t>
+  </si>
+  <si>
+    <t>Workforce</t>
+  </si>
+  <si>
+    <t>Includes costs associated with the workforce, including salary support and/or stipends, overhead, consultant fees, per diems, and travel expenses</t>
+  </si>
+  <si>
+    <t>Physical infrastructure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes costs to build, purchase, lease, or otherwise equip physical infrastucture, including laboratories, healthcare facilities, office space, and warehouses; also includes environmental monitoring equipment
+</t>
+  </si>
+  <si>
+    <t>Digital infrastructure</t>
+  </si>
+  <si>
+    <t>Includes costs of digital infrastructure and analytics infrastructure, such as web hosting, server space, and specialized software licenses</t>
+  </si>
+  <si>
+    <t>Civil infrastructure</t>
+  </si>
+  <si>
+    <t>Includes the costs of (select) civil infrastructure including resources used for transportation and WASH; note that explicit civil infrastructure costing is very minimal under the JEE, and only explicit investments (e.g., in vehicles for cold chain) are included</t>
+  </si>
+  <si>
+    <t>Media fees</t>
+  </si>
+  <si>
+    <t>World Health Organization. WHO-CHOICE estimates of cost for inpatient and outpatient health service delivery [Internet]. [cited 2023 Jul 28]. Available from: https://www.who.int/publications/m/item/who-choice-estimates-of-cost-for-inpatient-and-outpatient-health-service-delivery</t>
+  </si>
+  <si>
+    <t>Medical countermeasures and supplies for healthcare delivery</t>
+  </si>
+  <si>
+    <t>Includes the costs associated with the printing and dissemination of information via print (e.g., newsletters, magazines, newspapers, printed documents, posters, peer-reviewed journals), radio, television, or online, or to host a national hotline, also fees for media subscriptions</t>
+  </si>
+  <si>
+    <t>Includes costs of select medical countermeasures and supplies for healthcare delivery, including basic supplies for outbreak investigation and response, PPE for healthcare workers, and select medical countermeasures, including vaccines, antivirals, antimicrobials, and other biologics, drugs, or devices that may be used in the event of a potential public health emergency</t>
+  </si>
+  <si>
+    <t>US Food and Drug Administration. What are Medical Countermeasures? [Internet]. FDA. FDA; 2022 [cited 2023 Jan 13]. Available from: https://www.fda.gov/emergency-preparedness-and-response/about-mcmi/what-are-medical-countermeasures</t>
+  </si>
+  <si>
+    <t>Salary support and/or stipends, including overhead</t>
+  </si>
+  <si>
+    <t>Salaries, benefits, incentives, overhead for workers . Also includes costs associated with planning, meetings, and labor for healthcare delivery</t>
+  </si>
+  <si>
+    <t>Fees for domestic and international consultants</t>
+  </si>
+  <si>
+    <t>Consultant fees</t>
+  </si>
+  <si>
+    <t>Per diems and travel expenses</t>
+  </si>
+  <si>
+    <t>Per diems for salaried workers and travel expenses (domestic and international) for both salaried workers and consultants, also includes meeting expenses</t>
+  </si>
+  <si>
+    <t>Laboratories and laboratory equipment</t>
+  </si>
+  <si>
+    <t>Laboratory space (purchased or leased) and laboratory equipment</t>
+  </si>
+  <si>
+    <t>Healthcare facilities</t>
+  </si>
+  <si>
+    <t>Healthcare facility space (purchased or leased), including including treatment centers (not currently costed) and the construction or airborne isolation rooms</t>
+  </si>
+  <si>
+    <t>Office or other facility space</t>
+  </si>
+  <si>
+    <t>Office space, which may or may not be specialized (e.g., emergency operations centers and other coordinating centers). Includes costs of renting or purchasing and retrofitting physical office space, including basic office supplies like printers and fax machines</t>
+  </si>
+  <si>
+    <t>Warehouse or other storage space, including, for instance, storage space for a strategic national stockpile or other stockpile of national  or international importance</t>
+  </si>
+  <si>
+    <t>Warehouses or storage facilities</t>
+  </si>
+  <si>
+    <t>Equipment for environmental monitoring, including including biological, chemical, or radiological remote sensing equipment that could be used for remote monitoring</t>
+  </si>
+  <si>
+    <t>Environmental monitoring equipment</t>
+  </si>
+  <si>
+    <t>Digital or computational resources required for data collection, analysis, or reporting, including infrastructure to collect survey data online or via phone</t>
+  </si>
+  <si>
+    <t>Data analysis and analytics infrastructure</t>
+  </si>
+  <si>
+    <t>Computing resources beyond those included as general overhead fees for workforce, including additional computers or laptops, web hosting or cloud computing resources, or tablets</t>
+  </si>
+  <si>
+    <t>Computing resources</t>
+  </si>
+  <si>
+    <t>Transportation resources and resources to ensure a secure cold chain, including packaging and supplies needed to ship materials and/or specimen referral systems</t>
+  </si>
+  <si>
+    <t>Transportation and transport fees, including cold chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water infrastructure and resources, including costs associated with water, sanitation, and hygiene (WASH) resources </t>
+  </si>
+  <si>
+    <t>Water resources and WASH</t>
+  </si>
+  <si>
+    <t>Fees associated with the printing and dissemination of information via print (e.g., newsletters, magazines, newspapers, printed documents, posters, peer-reviewed journals), radio, television, or online, or to host a national hotline</t>
+  </si>
+  <si>
+    <t>Media operational costs</t>
+  </si>
+  <si>
+    <t>Subscriptions for various types of media including print (e.g., newsletters, magazines, newspapers), radio, or television</t>
+  </si>
+  <si>
+    <t>Media subscriptions</t>
+  </si>
+  <si>
+    <t>Select medical countermeasures, including vaccines, antivirals, antimicrobials, and other biologics, drugs, or devices that may be used in the event of a potential public health emergency</t>
+  </si>
+  <si>
+    <t>Medical countermeasures</t>
+  </si>
+  <si>
+    <t>Basic supplies for outbreak investigation and response, including supplies for vector control and sample collection and rapid response tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic supplies for outbreak investigation and response </t>
+  </si>
+  <si>
+    <t>Personal protective equipment, including supplies for biosafety incidents and emergency response</t>
+  </si>
+  <si>
+    <t>Personal protective equipment and basic supplies for infection prevention and control (IPC)</t>
+  </si>
+  <si>
+    <t>Added definitions for cost categories and subcategories</t>
+  </si>
+  <si>
+    <t>Adding documentation</t>
+  </si>
+  <si>
+    <t>The data dictionary was last updated on July 28, 2023</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +2027,7 @@
   <dimension ref="A2:W1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1903,7 +2051,7 @@
     </row>
     <row r="3" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>147</v>
+        <v>451</v>
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
@@ -1912,7 +2060,7 @@
     </row>
     <row r="4" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -1938,16 +2086,16 @@
     </row>
     <row r="7" spans="1:23" s="12" customFormat="1" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>134</v>
@@ -1958,22 +2106,22 @@
     </row>
     <row r="8" spans="1:23" s="17" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="D8" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="E8" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>155</v>
-      </c>
       <c r="F8" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
@@ -1995,22 +2143,22 @@
     </row>
     <row r="9" spans="1:23" s="17" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>159</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>160</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
@@ -2032,22 +2180,22 @@
     </row>
     <row r="10" spans="1:23" s="17" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C10" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D10" s="15" t="s">
+      <c r="E10" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>165</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>166</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
@@ -2069,22 +2217,22 @@
     </row>
     <row r="11" spans="1:23" s="17" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="E11" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>171</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>172</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
@@ -2106,22 +2254,22 @@
     </row>
     <row r="12" spans="1:23" s="17" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="C12" s="15" t="s">
+      <c r="E12" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>176</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>177</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
@@ -4208,8 +4356,8 @@
   </sheetPr>
   <dimension ref="A1:T999"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4238,7 +4386,7 @@
     </row>
     <row r="3" spans="1:20" s="19" customFormat="1" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>133</v>
@@ -4255,19 +4403,19 @@
     </row>
     <row r="4" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -4287,19 +4435,19 @@
     </row>
     <row r="5" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -4319,19 +4467,19 @@
     </row>
     <row r="6" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
@@ -4351,19 +4499,19 @@
     </row>
     <row r="7" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
@@ -4383,19 +4531,19 @@
     </row>
     <row r="8" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
@@ -4415,19 +4563,19 @@
     </row>
     <row r="9" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -4447,19 +4595,19 @@
     </row>
     <row r="10" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
@@ -4479,19 +4627,19 @@
     </row>
     <row r="11" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
@@ -4511,19 +4659,19 @@
     </row>
     <row r="12" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
@@ -4543,19 +4691,19 @@
     </row>
     <row r="13" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
@@ -4575,19 +4723,19 @@
     </row>
     <row r="14" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
@@ -4607,19 +4755,19 @@
     </row>
     <row r="15" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
@@ -4639,19 +4787,19 @@
     </row>
     <row r="16" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
@@ -4671,19 +4819,19 @@
     </row>
     <row r="17" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
@@ -4703,19 +4851,19 @@
     </row>
     <row r="18" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
@@ -4735,19 +4883,19 @@
     </row>
     <row r="19" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
@@ -4767,19 +4915,19 @@
     </row>
     <row r="20" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
@@ -4799,19 +4947,19 @@
     </row>
     <row r="21" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
@@ -4831,19 +4979,19 @@
     </row>
     <row r="22" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
@@ -4863,16 +5011,16 @@
     </row>
     <row r="23" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E23" s="30"/>
       <c r="F23" s="28"/>
@@ -4893,16 +5041,16 @@
     </row>
     <row r="24" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E24" s="30"/>
       <c r="F24" s="28"/>
@@ -4923,19 +5071,19 @@
     </row>
     <row r="25" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -4955,19 +5103,19 @@
     </row>
     <row r="26" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
@@ -4987,19 +5135,19 @@
     </row>
     <row r="27" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
@@ -5019,19 +5167,19 @@
     </row>
     <row r="28" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
@@ -5051,19 +5199,19 @@
     </row>
     <row r="29" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
@@ -5083,19 +5231,19 @@
     </row>
     <row r="30" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
@@ -5115,19 +5263,19 @@
     </row>
     <row r="31" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
@@ -5147,16 +5295,16 @@
     </row>
     <row r="32" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B32" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="C32" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="C32" s="26" t="s">
-        <v>248</v>
-      </c>
       <c r="D32" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E32" s="30"/>
       <c r="F32" s="28"/>
@@ -5177,16 +5325,16 @@
     </row>
     <row r="33" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E33" s="27"/>
       <c r="F33" s="28"/>
@@ -5207,19 +5355,19 @@
     </row>
     <row r="34" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F34" s="28"/>
       <c r="G34" s="28"/>
@@ -5239,16 +5387,16 @@
     </row>
     <row r="35" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>301</v>
+        <v>400</v>
       </c>
       <c r="E35" s="26"/>
       <c r="F35" s="28"/>
@@ -5269,16 +5417,16 @@
     </row>
     <row r="36" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>302</v>
+        <v>400</v>
       </c>
       <c r="E36" s="26"/>
       <c r="F36" s="28"/>
@@ -5299,16 +5447,16 @@
     </row>
     <row r="37" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E37" s="26"/>
       <c r="F37" s="28"/>
@@ -5329,16 +5477,16 @@
     </row>
     <row r="38" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E38" s="26"/>
       <c r="F38" s="28"/>
@@ -5359,16 +5507,16 @@
     </row>
     <row r="39" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E39" s="26"/>
       <c r="F39" s="28"/>
@@ -5389,16 +5537,16 @@
     </row>
     <row r="40" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40" s="28"/>
@@ -5419,16 +5567,16 @@
     </row>
     <row r="41" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E41" s="26"/>
       <c r="F41" s="28"/>
@@ -5449,16 +5597,16 @@
     </row>
     <row r="42" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E42" s="26"/>
       <c r="F42" s="28"/>
@@ -5479,16 +5627,16 @@
     </row>
     <row r="43" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E43" s="26"/>
       <c r="F43" s="28"/>
@@ -5509,16 +5657,16 @@
     </row>
     <row r="44" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E44" s="28"/>
       <c r="F44" s="28"/>
@@ -5539,16 +5687,16 @@
     </row>
     <row r="45" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E45" s="28"/>
       <c r="F45" s="28"/>
@@ -5569,16 +5717,16 @@
     </row>
     <row r="46" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
@@ -5599,16 +5747,16 @@
     </row>
     <row r="47" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E47" s="28"/>
       <c r="F47" s="28"/>
@@ -5629,19 +5777,19 @@
     </row>
     <row r="48" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D48" s="30" t="s">
+        <v>325</v>
+      </c>
+      <c r="E48" s="30" t="s">
         <v>328</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>331</v>
       </c>
       <c r="F48" s="28"/>
       <c r="G48" s="28"/>
@@ -5661,16 +5809,16 @@
     </row>
     <row r="49" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C49" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E49" s="28"/>
       <c r="F49" s="28"/>
@@ -5691,16 +5839,16 @@
     </row>
     <row r="50" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E50" s="28"/>
       <c r="F50" s="28"/>
@@ -5721,16 +5869,16 @@
     </row>
     <row r="51" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E51" s="28"/>
       <c r="F51" s="28"/>
@@ -5751,19 +5899,19 @@
     </row>
     <row r="52" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="B52" s="29" t="s">
-        <v>174</v>
-      </c>
       <c r="C52" s="26" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E52" s="30" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F52" s="28"/>
       <c r="G52" s="28"/>
@@ -5783,266 +5931,266 @@
     </row>
     <row r="53" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="54" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="E54" s="30" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="55" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="56" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E56" s="30"/>
     </row>
     <row r="57" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E57" s="30"/>
     </row>
     <row r="58" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E58" s="30"/>
     </row>
     <row r="59" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E59" s="30"/>
     </row>
     <row r="60" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C60" s="29" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="30" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E60" s="30"/>
     </row>
     <row r="61" spans="1:20" s="29" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B61" s="29" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C61" s="29" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D61" s="30" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="62" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B62" s="29" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D62" s="30" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="63" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B63" s="29" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C63" s="29" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D63" s="30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E63" s="30"/>
     </row>
     <row r="64" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B64" s="29" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E64" s="30"/>
     </row>
     <row r="65" spans="1:5" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B65" s="29" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E65" s="30"/>
     </row>
     <row r="66" spans="1:5" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B66" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D66" s="30" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E66" s="30"/>
     </row>
     <row r="67" spans="1:5" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E67" s="30"/>
     </row>
     <row r="68" spans="1:5" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B68" s="29" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D68" s="30" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E68" s="30"/>
     </row>
     <row r="69" spans="1:5" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E69" s="30"/>
     </row>
@@ -6991,10 +7139,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S1000"/>
+  <dimension ref="A1:S1023"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7039,19 +7187,19 @@
     </row>
     <row r="4" spans="1:19" s="41" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C4" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4" s="34" t="s">
         <v>312</v>
       </c>
-      <c r="D4" s="34" t="s">
-        <v>315</v>
-      </c>
       <c r="E4" s="34" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F4" s="35"/>
       <c r="G4" s="35"/>
@@ -7070,19 +7218,19 @@
     </row>
     <row r="5" spans="1:19" s="41" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C5" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>313</v>
       </c>
-      <c r="D5" s="34" t="s">
-        <v>316</v>
-      </c>
       <c r="E5" s="34" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F5" s="35"/>
       <c r="G5" s="35"/>
@@ -7101,19 +7249,19 @@
     </row>
     <row r="6" spans="1:19" s="41" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C6" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="E6" s="34" t="s">
         <v>314</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>311</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>317</v>
       </c>
       <c r="F6" s="35"/>
       <c r="G6" s="35"/>
@@ -7130,20 +7278,20 @@
       <c r="R6" s="35"/>
       <c r="S6" s="35"/>
     </row>
-    <row r="7" spans="1:19" s="41" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>336</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>156</v>
+    <row r="7" spans="1:19" s="41" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>401</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>386</v>
-      </c>
-      <c r="E7" s="35"/>
+        <v>402</v>
+      </c>
+      <c r="E7" s="34"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
@@ -7159,20 +7307,20 @@
       <c r="R7" s="35"/>
       <c r="S7" s="35"/>
     </row>
-    <row r="8" spans="1:19" s="41" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>336</v>
+    <row r="8" spans="1:19" s="41" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>279</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>398</v>
-      </c>
-      <c r="E8" s="35"/>
+        <v>404</v>
+      </c>
+      <c r="E8" s="34"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
@@ -7188,536 +7336,690 @@
       <c r="R8" s="35"/>
       <c r="S8" s="35"/>
     </row>
-    <row r="9" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>336</v>
+    <row r="9" spans="1:19" s="41" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>279</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>387</v>
+        <v>405</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>388</v>
-      </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="42"/>
-      <c r="S9" s="42"/>
-    </row>
-    <row r="10" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>336</v>
+        <v>406</v>
+      </c>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+    </row>
+    <row r="10" spans="1:19" s="41" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>279</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>389</v>
-      </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="42"/>
-    </row>
-    <row r="11" spans="1:19" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>336</v>
+        <v>408</v>
+      </c>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+    </row>
+    <row r="11" spans="1:19" s="41" customFormat="1" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>279</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>392</v>
+        <v>409</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>391</v>
-      </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
-    </row>
-    <row r="12" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>336</v>
+        <v>412</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>410</v>
+      </c>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+    </row>
+    <row r="12" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>279</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>393</v>
+        <v>411</v>
       </c>
       <c r="D12" s="34" t="s">
+        <v>413</v>
+      </c>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+    </row>
+    <row r="13" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>415</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>416</v>
+      </c>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+    </row>
+    <row r="14" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>418</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>417</v>
+      </c>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+    </row>
+    <row r="15" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>420</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+    </row>
+    <row r="16" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>422</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+    </row>
+    <row r="17" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>423</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>424</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+    </row>
+    <row r="18" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>425</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>426</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+    </row>
+    <row r="19" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>428</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>427</v>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+    </row>
+    <row r="20" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>430</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>429</v>
+      </c>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+    </row>
+    <row r="21" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>432</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>431</v>
+      </c>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+    </row>
+    <row r="22" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>434</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>433</v>
+      </c>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+    </row>
+    <row r="23" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>436</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>435</v>
+      </c>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+    </row>
+    <row r="24" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>438</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="E24" s="34"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+    </row>
+    <row r="25" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>440</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>439</v>
+      </c>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+    </row>
+    <row r="26" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>442</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35"/>
+    </row>
+    <row r="27" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>444</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>443</v>
+      </c>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+    </row>
+    <row r="28" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>445</v>
+      </c>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+    </row>
+    <row r="29" spans="1:19" s="41" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>448</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>447</v>
+      </c>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="35"/>
+      <c r="S29" s="35"/>
+    </row>
+    <row r="30" spans="1:19" s="41" customFormat="1" ht="121" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>383</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="35"/>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="35"/>
+      <c r="S30" s="35"/>
+    </row>
+    <row r="31" spans="1:19" s="41" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="C31" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
-    </row>
-    <row r="13" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>336</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>400</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>401</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>402</v>
-      </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
-    </row>
-    <row r="14" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
-    </row>
-    <row r="15" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-    </row>
-    <row r="16" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
-    </row>
-    <row r="17" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
-    </row>
-    <row r="18" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
-      <c r="S18" s="42"/>
-    </row>
-    <row r="19" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
-    </row>
-    <row r="20" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
-      <c r="S20" s="42"/>
-    </row>
-    <row r="21" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="42"/>
-      <c r="S21" s="42"/>
-    </row>
-    <row r="22" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="42"/>
-    </row>
-    <row r="23" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="42"/>
-      <c r="S23" s="42"/>
-    </row>
-    <row r="24" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
-    </row>
-    <row r="25" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="42"/>
-      <c r="S25" s="42"/>
-    </row>
-    <row r="26" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="42"/>
-    </row>
-    <row r="27" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
-    </row>
-    <row r="28" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="42"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="42"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="42"/>
-      <c r="S28" s="42"/>
-    </row>
-    <row r="29" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="42"/>
-      <c r="S29" s="42"/>
-    </row>
-    <row r="30" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="42"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="42"/>
-      <c r="S30" s="42"/>
-    </row>
-    <row r="31" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="42"/>
+      <c r="D31" s="34" t="s">
+        <v>395</v>
+      </c>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="35"/>
+      <c r="S31" s="35"/>
     </row>
     <row r="32" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
+      <c r="A32" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>384</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>385</v>
+      </c>
       <c r="E32" s="42"/>
       <c r="F32" s="42"/>
       <c r="G32" s="42"/>
@@ -7735,10 +8037,18 @@
       <c r="S32" s="42"/>
     </row>
     <row r="33" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
+      <c r="A33" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>387</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>386</v>
+      </c>
       <c r="E33" s="42"/>
       <c r="F33" s="42"/>
       <c r="G33" s="42"/>
@@ -7755,11 +8065,19 @@
       <c r="R33" s="42"/>
       <c r="S33" s="42"/>
     </row>
-    <row r="34" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
+    <row r="34" spans="1:19" ht="97" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>389</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>388</v>
+      </c>
       <c r="E34" s="42"/>
       <c r="F34" s="42"/>
       <c r="G34" s="42"/>
@@ -7777,10 +8095,18 @@
       <c r="S34" s="42"/>
     </row>
     <row r="35" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
+      <c r="A35" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B35" s="43" t="s">
+        <v>333</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>390</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>391</v>
+      </c>
       <c r="E35" s="42"/>
       <c r="F35" s="42"/>
       <c r="G35" s="42"/>
@@ -7798,11 +8124,21 @@
       <c r="S35" s="42"/>
     </row>
     <row r="36" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="42"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
+      <c r="A36" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>333</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>397</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>398</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>399</v>
+      </c>
       <c r="F36" s="42"/>
       <c r="G36" s="42"/>
       <c r="H36" s="42"/>
@@ -8133,7 +8469,7 @@
       <c r="R51" s="42"/>
       <c r="S51" s="42"/>
     </row>
-    <row r="52" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="42"/>
       <c r="B52" s="42"/>
       <c r="C52" s="42"/>
@@ -8154,7 +8490,7 @@
       <c r="R52" s="42"/>
       <c r="S52" s="42"/>
     </row>
-    <row r="53" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="42"/>
       <c r="B53" s="42"/>
       <c r="C53" s="42"/>
@@ -8175,33 +8511,493 @@
       <c r="R53" s="42"/>
       <c r="S53" s="42"/>
     </row>
-    <row r="54" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="42"/>
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="42"/>
+      <c r="J54" s="42"/>
+      <c r="K54" s="42"/>
+      <c r="L54" s="42"/>
+      <c r="M54" s="42"/>
+      <c r="N54" s="42"/>
+      <c r="O54" s="42"/>
+      <c r="P54" s="42"/>
+      <c r="Q54" s="42"/>
+      <c r="R54" s="42"/>
+      <c r="S54" s="42"/>
+    </row>
+    <row r="55" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="42"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="42"/>
+      <c r="I55" s="42"/>
+      <c r="J55" s="42"/>
+      <c r="K55" s="42"/>
+      <c r="L55" s="42"/>
+      <c r="M55" s="42"/>
+      <c r="N55" s="42"/>
+      <c r="O55" s="42"/>
+      <c r="P55" s="42"/>
+      <c r="Q55" s="42"/>
+      <c r="R55" s="42"/>
+      <c r="S55" s="42"/>
+    </row>
+    <row r="56" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="42"/>
+      <c r="B56" s="42"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="42"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="42"/>
+      <c r="H56" s="42"/>
+      <c r="I56" s="42"/>
+      <c r="J56" s="42"/>
+      <c r="K56" s="42"/>
+      <c r="L56" s="42"/>
+      <c r="M56" s="42"/>
+      <c r="N56" s="42"/>
+      <c r="O56" s="42"/>
+      <c r="P56" s="42"/>
+      <c r="Q56" s="42"/>
+      <c r="R56" s="42"/>
+      <c r="S56" s="42"/>
+    </row>
+    <row r="57" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="42"/>
+      <c r="B57" s="42"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="42"/>
+      <c r="I57" s="42"/>
+      <c r="J57" s="42"/>
+      <c r="K57" s="42"/>
+      <c r="L57" s="42"/>
+      <c r="M57" s="42"/>
+      <c r="N57" s="42"/>
+      <c r="O57" s="42"/>
+      <c r="P57" s="42"/>
+      <c r="Q57" s="42"/>
+      <c r="R57" s="42"/>
+      <c r="S57" s="42"/>
+    </row>
+    <row r="58" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="42"/>
+      <c r="B58" s="42"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="42"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="42"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="42"/>
+      <c r="J58" s="42"/>
+      <c r="K58" s="42"/>
+      <c r="L58" s="42"/>
+      <c r="M58" s="42"/>
+      <c r="N58" s="42"/>
+      <c r="O58" s="42"/>
+      <c r="P58" s="42"/>
+      <c r="Q58" s="42"/>
+      <c r="R58" s="42"/>
+      <c r="S58" s="42"/>
+    </row>
+    <row r="59" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="42"/>
+      <c r="B59" s="42"/>
+      <c r="C59" s="42"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
+      <c r="H59" s="42"/>
+      <c r="I59" s="42"/>
+      <c r="J59" s="42"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="42"/>
+      <c r="M59" s="42"/>
+      <c r="N59" s="42"/>
+      <c r="O59" s="42"/>
+      <c r="P59" s="42"/>
+      <c r="Q59" s="42"/>
+      <c r="R59" s="42"/>
+      <c r="S59" s="42"/>
+    </row>
+    <row r="60" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="42"/>
+      <c r="B60" s="42"/>
+      <c r="C60" s="42"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
+      <c r="H60" s="42"/>
+      <c r="I60" s="42"/>
+      <c r="J60" s="42"/>
+      <c r="K60" s="42"/>
+      <c r="L60" s="42"/>
+      <c r="M60" s="42"/>
+      <c r="N60" s="42"/>
+      <c r="O60" s="42"/>
+      <c r="P60" s="42"/>
+      <c r="Q60" s="42"/>
+      <c r="R60" s="42"/>
+      <c r="S60" s="42"/>
+    </row>
+    <row r="61" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="42"/>
+      <c r="B61" s="42"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="42"/>
+      <c r="I61" s="42"/>
+      <c r="J61" s="42"/>
+      <c r="K61" s="42"/>
+      <c r="L61" s="42"/>
+      <c r="M61" s="42"/>
+      <c r="N61" s="42"/>
+      <c r="O61" s="42"/>
+      <c r="P61" s="42"/>
+      <c r="Q61" s="42"/>
+      <c r="R61" s="42"/>
+      <c r="S61" s="42"/>
+    </row>
+    <row r="62" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="42"/>
+      <c r="B62" s="42"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="42"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="42"/>
+      <c r="H62" s="42"/>
+      <c r="I62" s="42"/>
+      <c r="J62" s="42"/>
+      <c r="K62" s="42"/>
+      <c r="L62" s="42"/>
+      <c r="M62" s="42"/>
+      <c r="N62" s="42"/>
+      <c r="O62" s="42"/>
+      <c r="P62" s="42"/>
+      <c r="Q62" s="42"/>
+      <c r="R62" s="42"/>
+      <c r="S62" s="42"/>
+    </row>
+    <row r="63" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="42"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="42"/>
+      <c r="J63" s="42"/>
+      <c r="K63" s="42"/>
+      <c r="L63" s="42"/>
+      <c r="M63" s="42"/>
+      <c r="N63" s="42"/>
+      <c r="O63" s="42"/>
+      <c r="P63" s="42"/>
+      <c r="Q63" s="42"/>
+      <c r="R63" s="42"/>
+      <c r="S63" s="42"/>
+    </row>
+    <row r="64" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="42"/>
+      <c r="B64" s="42"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="42"/>
+      <c r="I64" s="42"/>
+      <c r="J64" s="42"/>
+      <c r="K64" s="42"/>
+      <c r="L64" s="42"/>
+      <c r="M64" s="42"/>
+      <c r="N64" s="42"/>
+      <c r="O64" s="42"/>
+      <c r="P64" s="42"/>
+      <c r="Q64" s="42"/>
+      <c r="R64" s="42"/>
+      <c r="S64" s="42"/>
+    </row>
+    <row r="65" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="42"/>
+      <c r="B65" s="42"/>
+      <c r="C65" s="42"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="42"/>
+      <c r="H65" s="42"/>
+      <c r="I65" s="42"/>
+      <c r="J65" s="42"/>
+      <c r="K65" s="42"/>
+      <c r="L65" s="42"/>
+      <c r="M65" s="42"/>
+      <c r="N65" s="42"/>
+      <c r="O65" s="42"/>
+      <c r="P65" s="42"/>
+      <c r="Q65" s="42"/>
+      <c r="R65" s="42"/>
+      <c r="S65" s="42"/>
+    </row>
+    <row r="66" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="42"/>
+      <c r="B66" s="42"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="42"/>
+      <c r="I66" s="42"/>
+      <c r="J66" s="42"/>
+      <c r="K66" s="42"/>
+      <c r="L66" s="42"/>
+      <c r="M66" s="42"/>
+      <c r="N66" s="42"/>
+      <c r="O66" s="42"/>
+      <c r="P66" s="42"/>
+      <c r="Q66" s="42"/>
+      <c r="R66" s="42"/>
+      <c r="S66" s="42"/>
+    </row>
+    <row r="67" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="42"/>
+      <c r="B67" s="42"/>
+      <c r="C67" s="42"/>
+      <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="42"/>
+      <c r="H67" s="42"/>
+      <c r="I67" s="42"/>
+      <c r="J67" s="42"/>
+      <c r="K67" s="42"/>
+      <c r="L67" s="42"/>
+      <c r="M67" s="42"/>
+      <c r="N67" s="42"/>
+      <c r="O67" s="42"/>
+      <c r="P67" s="42"/>
+      <c r="Q67" s="42"/>
+      <c r="R67" s="42"/>
+      <c r="S67" s="42"/>
+    </row>
+    <row r="68" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="42"/>
+      <c r="B68" s="42"/>
+      <c r="C68" s="42"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="42"/>
+      <c r="H68" s="42"/>
+      <c r="I68" s="42"/>
+      <c r="J68" s="42"/>
+      <c r="K68" s="42"/>
+      <c r="L68" s="42"/>
+      <c r="M68" s="42"/>
+      <c r="N68" s="42"/>
+      <c r="O68" s="42"/>
+      <c r="P68" s="42"/>
+      <c r="Q68" s="42"/>
+      <c r="R68" s="42"/>
+      <c r="S68" s="42"/>
+    </row>
+    <row r="69" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="42"/>
+      <c r="B69" s="42"/>
+      <c r="C69" s="42"/>
+      <c r="D69" s="42"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
+      <c r="H69" s="42"/>
+      <c r="I69" s="42"/>
+      <c r="J69" s="42"/>
+      <c r="K69" s="42"/>
+      <c r="L69" s="42"/>
+      <c r="M69" s="42"/>
+      <c r="N69" s="42"/>
+      <c r="O69" s="42"/>
+      <c r="P69" s="42"/>
+      <c r="Q69" s="42"/>
+      <c r="R69" s="42"/>
+      <c r="S69" s="42"/>
+    </row>
+    <row r="70" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="42"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
+      <c r="H70" s="42"/>
+      <c r="I70" s="42"/>
+      <c r="J70" s="42"/>
+      <c r="K70" s="42"/>
+      <c r="L70" s="42"/>
+      <c r="M70" s="42"/>
+      <c r="N70" s="42"/>
+      <c r="O70" s="42"/>
+      <c r="P70" s="42"/>
+      <c r="Q70" s="42"/>
+      <c r="R70" s="42"/>
+      <c r="S70" s="42"/>
+    </row>
+    <row r="71" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="42"/>
+      <c r="B71" s="42"/>
+      <c r="C71" s="42"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="42"/>
+      <c r="F71" s="42"/>
+      <c r="G71" s="42"/>
+      <c r="H71" s="42"/>
+      <c r="I71" s="42"/>
+      <c r="J71" s="42"/>
+      <c r="K71" s="42"/>
+      <c r="L71" s="42"/>
+      <c r="M71" s="42"/>
+      <c r="N71" s="42"/>
+      <c r="O71" s="42"/>
+      <c r="P71" s="42"/>
+      <c r="Q71" s="42"/>
+      <c r="R71" s="42"/>
+      <c r="S71" s="42"/>
+    </row>
+    <row r="72" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="42"/>
+      <c r="B72" s="42"/>
+      <c r="C72" s="42"/>
+      <c r="D72" s="42"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="42"/>
+      <c r="G72" s="42"/>
+      <c r="H72" s="42"/>
+      <c r="I72" s="42"/>
+      <c r="J72" s="42"/>
+      <c r="K72" s="42"/>
+      <c r="L72" s="42"/>
+      <c r="M72" s="42"/>
+      <c r="N72" s="42"/>
+      <c r="O72" s="42"/>
+      <c r="P72" s="42"/>
+      <c r="Q72" s="42"/>
+      <c r="R72" s="42"/>
+      <c r="S72" s="42"/>
+    </row>
+    <row r="73" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="42"/>
+      <c r="B73" s="42"/>
+      <c r="C73" s="42"/>
+      <c r="D73" s="42"/>
+      <c r="E73" s="42"/>
+      <c r="F73" s="42"/>
+      <c r="G73" s="42"/>
+      <c r="H73" s="42"/>
+      <c r="I73" s="42"/>
+      <c r="J73" s="42"/>
+      <c r="K73" s="42"/>
+      <c r="L73" s="42"/>
+      <c r="M73" s="42"/>
+      <c r="N73" s="42"/>
+      <c r="O73" s="42"/>
+      <c r="P73" s="42"/>
+      <c r="Q73" s="42"/>
+      <c r="R73" s="42"/>
+      <c r="S73" s="42"/>
+    </row>
+    <row r="74" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="42"/>
+      <c r="B74" s="42"/>
+      <c r="C74" s="42"/>
+      <c r="D74" s="42"/>
+      <c r="E74" s="42"/>
+      <c r="F74" s="42"/>
+      <c r="G74" s="42"/>
+      <c r="H74" s="42"/>
+      <c r="I74" s="42"/>
+      <c r="J74" s="42"/>
+      <c r="K74" s="42"/>
+      <c r="L74" s="42"/>
+      <c r="M74" s="42"/>
+      <c r="N74" s="42"/>
+      <c r="O74" s="42"/>
+      <c r="P74" s="42"/>
+      <c r="Q74" s="42"/>
+      <c r="R74" s="42"/>
+      <c r="S74" s="42"/>
+    </row>
+    <row r="75" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="42"/>
+      <c r="B75" s="42"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="42"/>
+      <c r="I75" s="42"/>
+      <c r="J75" s="42"/>
+      <c r="K75" s="42"/>
+      <c r="L75" s="42"/>
+      <c r="M75" s="42"/>
+      <c r="N75" s="42"/>
+      <c r="O75" s="42"/>
+      <c r="P75" s="42"/>
+      <c r="Q75" s="42"/>
+      <c r="R75" s="42"/>
+      <c r="S75" s="42"/>
+    </row>
+    <row r="76" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="42"/>
+      <c r="B76" s="42"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
+      <c r="H76" s="42"/>
+      <c r="I76" s="42"/>
+      <c r="J76" s="42"/>
+      <c r="K76" s="42"/>
+      <c r="L76" s="42"/>
+      <c r="M76" s="42"/>
+      <c r="N76" s="42"/>
+      <c r="O76" s="42"/>
+      <c r="P76" s="42"/>
+      <c r="Q76" s="42"/>
+      <c r="R76" s="42"/>
+      <c r="S76" s="42"/>
+    </row>
+    <row r="77" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9122,6 +9918,29 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E2"/>
@@ -9140,7 +9959,7 @@
   <dimension ref="A1:S999"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9187,16 +10006,16 @@
         <v>45114</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -9214,11 +10033,21 @@
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="32">
+        <v>45135</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>155</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>

</xml_diff>

<commit_message>
recode internet costs as subcategory to clarify definition and more clearly exclude from what is already costed in 60% overhead
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC96A000-EF53-C641-AA38-A147322CADAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0104A6C-CB04-FA43-9D30-5272F324AE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -2027,7 +2027,7 @@
   <dimension ref="A2:W1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4356,7 +4356,7 @@
   </sheetPr>
   <dimension ref="A1:T999"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -7142,7 +7142,7 @@
   <dimension ref="A1:S1023"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
first pass tagging of health emergency corps levels, still needs review, cleanup, and standardiziation
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/IHR-costing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3867DA4E-40E3-784C-86B0-82A3E5F2B6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2059D3-F4B3-FB49-836C-D39C5A4C4EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1260" yWindow="5220" windowWidth="29780" windowHeight="16820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="467">
   <si>
     <t>Text</t>
   </si>
@@ -1259,198 +1259,286 @@
     <t>The action (activity, investment, etc) required to address the requirement</t>
   </si>
   <si>
-    <t xml:space="preserve">Population
+    <t>National</t>
+  </si>
+  <si>
+    <t>The central government or central geopolitical unit</t>
+  </si>
+  <si>
+    <t>Defines country geopolitical organization and/or the level of implementation at which a given action needs to happen (e.g., once nationally, once per intermediate area, or once per health facility, or scaled linearly by population size). For the purposes of costing IHR implementation, these are the administrative units that support public health efforts such as biosurveillance or emergency response. See "Definitions" tab for additional defintions.</t>
+  </si>
+  <si>
+    <t>Additional healthcare workers (doctors, nurses, and midwives)</t>
+  </si>
+  <si>
+    <t>The additional healthcare workers, including doctors, nurses, and midwives, intended to be costed beyond the current in-country human resource capacity.</t>
+  </si>
+  <si>
+    <t>JEE 3.0 specifies that "The recommended density of doctors, nurses and midwives per 1000 population for operational routine services is 4.45 plus 30% surge capacity"</t>
+  </si>
+  <si>
+    <t>The category of the cost based on the cost categories defined by GHSS. Please see methods documentation and definitions tab for more detailed definitions</t>
+  </si>
+  <si>
+    <t>Workforce</t>
+  </si>
+  <si>
+    <t>Includes costs associated with the workforce, including salary support and/or stipends, overhead, consultant fees, per diems, and travel expenses</t>
+  </si>
+  <si>
+    <t>Physical infrastructure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes costs to build, purchase, lease, or otherwise equip physical infrastucture, including laboratories, healthcare facilities, office space, and warehouses; also includes environmental monitoring equipment
+</t>
+  </si>
+  <si>
+    <t>Digital infrastructure</t>
+  </si>
+  <si>
+    <t>Includes costs of digital infrastructure and analytics infrastructure, such as web hosting, server space, and specialized software licenses</t>
+  </si>
+  <si>
+    <t>Civil infrastructure</t>
+  </si>
+  <si>
+    <t>Includes the costs of (select) civil infrastructure including resources used for transportation and WASH; note that explicit civil infrastructure costing is very minimal under the JEE, and only explicit investments (e.g., in vehicles for cold chain) are included</t>
+  </si>
+  <si>
+    <t>Media fees</t>
+  </si>
+  <si>
+    <t>World Health Organization. WHO-CHOICE estimates of cost for inpatient and outpatient health service delivery [Internet]. [cited 2023 Jul 28]. Available from: https://www.who.int/publications/m/item/who-choice-estimates-of-cost-for-inpatient-and-outpatient-health-service-delivery</t>
+  </si>
+  <si>
+    <t>Medical countermeasures and supplies for healthcare delivery</t>
+  </si>
+  <si>
+    <t>Includes the costs associated with the printing and dissemination of information via print (e.g., newsletters, magazines, newspapers, printed documents, posters, peer-reviewed journals), radio, television, or online, or to host a national hotline, also fees for media subscriptions</t>
+  </si>
+  <si>
+    <t>Includes costs of select medical countermeasures and supplies for healthcare delivery, including basic supplies for outbreak investigation and response, PPE for healthcare workers, and select medical countermeasures, including vaccines, antivirals, antimicrobials, and other biologics, drugs, or devices that may be used in the event of a potential public health emergency</t>
+  </si>
+  <si>
+    <t>US Food and Drug Administration. What are Medical Countermeasures? [Internet]. FDA. FDA; 2022 [cited 2023 Jan 13]. Available from: https://www.fda.gov/emergency-preparedness-and-response/about-mcmi/what-are-medical-countermeasures</t>
+  </si>
+  <si>
+    <t>Salary support and/or stipends, including overhead</t>
+  </si>
+  <si>
+    <t>Salaries, benefits, incentives, overhead for workers . Also includes costs associated with planning, meetings, and labor for healthcare delivery</t>
+  </si>
+  <si>
+    <t>Fees for domestic and international consultants</t>
+  </si>
+  <si>
+    <t>Consultant fees</t>
+  </si>
+  <si>
+    <t>Per diems and travel expenses</t>
+  </si>
+  <si>
+    <t>Per diems for salaried workers and travel expenses (domestic and international) for both salaried workers and consultants, also includes meeting expenses</t>
+  </si>
+  <si>
+    <t>Laboratories and laboratory equipment</t>
+  </si>
+  <si>
+    <t>Laboratory space (purchased or leased) and laboratory equipment</t>
+  </si>
+  <si>
+    <t>Healthcare facilities</t>
+  </si>
+  <si>
+    <t>Healthcare facility space (purchased or leased), including including treatment centers (not currently costed) and the construction or airborne isolation rooms</t>
+  </si>
+  <si>
+    <t>Office or other facility space</t>
+  </si>
+  <si>
+    <t>Office space, which may or may not be specialized (e.g., emergency operations centers and other coordinating centers). Includes costs of renting or purchasing and retrofitting physical office space, including basic office supplies like printers and fax machines</t>
+  </si>
+  <si>
+    <t>Warehouse or other storage space, including, for instance, storage space for a strategic national stockpile or other stockpile of national  or international importance</t>
+  </si>
+  <si>
+    <t>Warehouses or storage facilities</t>
+  </si>
+  <si>
+    <t>Equipment for environmental monitoring, including including biological, chemical, or radiological remote sensing equipment that could be used for remote monitoring</t>
+  </si>
+  <si>
+    <t>Environmental monitoring equipment</t>
+  </si>
+  <si>
+    <t>Digital or computational resources required for data collection, analysis, or reporting, including infrastructure to collect survey data online or via phone</t>
+  </si>
+  <si>
+    <t>Data analysis and analytics infrastructure</t>
+  </si>
+  <si>
+    <t>Computing resources beyond those included as general overhead fees for workforce, including additional computers or laptops, web hosting or cloud computing resources, or tablets</t>
+  </si>
+  <si>
+    <t>Computing resources</t>
+  </si>
+  <si>
+    <t>Transportation resources and resources to ensure a secure cold chain, including packaging and supplies needed to ship materials and/or specimen referral systems</t>
+  </si>
+  <si>
+    <t>Transportation and transport fees, including cold chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water infrastructure and resources, including costs associated with water, sanitation, and hygiene (WASH) resources </t>
+  </si>
+  <si>
+    <t>Water resources and WASH</t>
+  </si>
+  <si>
+    <t>Fees associated with the printing and dissemination of information via print (e.g., newsletters, magazines, newspapers, printed documents, posters, peer-reviewed journals), radio, television, or online, or to host a national hotline</t>
+  </si>
+  <si>
+    <t>Subscriptions for various types of media including print (e.g., newsletters, magazines, newspapers), radio, or television</t>
+  </si>
+  <si>
+    <t>Media subscriptions</t>
+  </si>
+  <si>
+    <t>Select medical countermeasures, including vaccines, antivirals, antimicrobials, and other biologics, drugs, or devices that may be used in the event of a potential public health emergency</t>
+  </si>
+  <si>
+    <t>Medical countermeasures</t>
+  </si>
+  <si>
+    <t>Basic supplies for outbreak investigation and response, including supplies for vector control and sample collection and rapid response tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic supplies for outbreak investigation and response </t>
+  </si>
+  <si>
+    <t>Personal protective equipment, including supplies for biosafety incidents and emergency response</t>
+  </si>
+  <si>
+    <t>Personal protective equipment and basic supplies for infection prevention and control (IPC)</t>
+  </si>
+  <si>
+    <t>Added definitions for cost categories and subcategories</t>
+  </si>
+  <si>
+    <t>Adding documentation</t>
+  </si>
+  <si>
+    <t>Media distribution costs</t>
+  </si>
+  <si>
+    <t>Revised select names and definitions of cost subcategories</t>
+  </si>
+  <si>
+    <t>The data dictionary was last updated on October 27, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added additional field in line_item table for </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>One of:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Population
 National
 Intermediate
 Local
 PoE
 Health facility
-Additional healthcare workers (doctors, nurses, and midwives) </t>
-  </si>
-  <si>
-    <t>National</t>
-  </si>
-  <si>
-    <t>The central government or central geopolitical unit</t>
-  </si>
-  <si>
-    <t>Defines country geopolitical organization and/or the level of implementation at which a given action needs to happen (e.g., once nationally, once per intermediate area, or once per health facility, or scaled linearly by population size). For the purposes of costing IHR implementation, these are the administrative units that support public health efforts such as biosurveillance or emergency response. See "Definitions" tab for additional defintions.</t>
-  </si>
-  <si>
-    <t>Additional healthcare workers (doctors, nurses, and midwives)</t>
-  </si>
-  <si>
-    <t>The additional healthcare workers, including doctors, nurses, and midwives, intended to be costed beyond the current in-country human resource capacity.</t>
-  </si>
-  <si>
-    <t>JEE 3.0 specifies that "The recommended density of doctors, nurses and midwives per 1000 population for operational routine services is 4.45 plus 30% surge capacity"</t>
-  </si>
-  <si>
-    <t>The category of the cost based on the cost categories defined by GHSS. Please see methods documentation and definitions tab for more detailed definitions</t>
-  </si>
-  <si>
-    <t>Workforce</t>
-  </si>
-  <si>
-    <t>Includes costs associated with the workforce, including salary support and/or stipends, overhead, consultant fees, per diems, and travel expenses</t>
-  </si>
-  <si>
-    <t>Physical infrastructure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Includes costs to build, purchase, lease, or otherwise equip physical infrastucture, including laboratories, healthcare facilities, office space, and warehouses; also includes environmental monitoring equipment
-</t>
-  </si>
-  <si>
-    <t>Digital infrastructure</t>
-  </si>
-  <si>
-    <t>Includes costs of digital infrastructure and analytics infrastructure, such as web hosting, server space, and specialized software licenses</t>
-  </si>
-  <si>
-    <t>Civil infrastructure</t>
-  </si>
-  <si>
-    <t>Includes the costs of (select) civil infrastructure including resources used for transportation and WASH; note that explicit civil infrastructure costing is very minimal under the JEE, and only explicit investments (e.g., in vehicles for cold chain) are included</t>
-  </si>
-  <si>
-    <t>Media fees</t>
-  </si>
-  <si>
-    <t>World Health Organization. WHO-CHOICE estimates of cost for inpatient and outpatient health service delivery [Internet]. [cited 2023 Jul 28]. Available from: https://www.who.int/publications/m/item/who-choice-estimates-of-cost-for-inpatient-and-outpatient-health-service-delivery</t>
-  </si>
-  <si>
-    <t>Medical countermeasures and supplies for healthcare delivery</t>
-  </si>
-  <si>
-    <t>Includes the costs associated with the printing and dissemination of information via print (e.g., newsletters, magazines, newspapers, printed documents, posters, peer-reviewed journals), radio, television, or online, or to host a national hotline, also fees for media subscriptions</t>
-  </si>
-  <si>
-    <t>Includes costs of select medical countermeasures and supplies for healthcare delivery, including basic supplies for outbreak investigation and response, PPE for healthcare workers, and select medical countermeasures, including vaccines, antivirals, antimicrobials, and other biologics, drugs, or devices that may be used in the event of a potential public health emergency</t>
-  </si>
-  <si>
-    <t>US Food and Drug Administration. What are Medical Countermeasures? [Internet]. FDA. FDA; 2022 [cited 2023 Jan 13]. Available from: https://www.fda.gov/emergency-preparedness-and-response/about-mcmi/what-are-medical-countermeasures</t>
-  </si>
-  <si>
-    <t>Salary support and/or stipends, including overhead</t>
-  </si>
-  <si>
-    <t>Salaries, benefits, incentives, overhead for workers . Also includes costs associated with planning, meetings, and labor for healthcare delivery</t>
-  </si>
-  <si>
-    <t>Fees for domestic and international consultants</t>
-  </si>
-  <si>
-    <t>Consultant fees</t>
-  </si>
-  <si>
-    <t>Per diems and travel expenses</t>
-  </si>
-  <si>
-    <t>Per diems for salaried workers and travel expenses (domestic and international) for both salaried workers and consultants, also includes meeting expenses</t>
-  </si>
-  <si>
-    <t>Laboratories and laboratory equipment</t>
-  </si>
-  <si>
-    <t>Laboratory space (purchased or leased) and laboratory equipment</t>
-  </si>
-  <si>
-    <t>Healthcare facilities</t>
-  </si>
-  <si>
-    <t>Healthcare facility space (purchased or leased), including including treatment centers (not currently costed) and the construction or airborne isolation rooms</t>
-  </si>
-  <si>
-    <t>Office or other facility space</t>
-  </si>
-  <si>
-    <t>Office space, which may or may not be specialized (e.g., emergency operations centers and other coordinating centers). Includes costs of renting or purchasing and retrofitting physical office space, including basic office supplies like printers and fax machines</t>
-  </si>
-  <si>
-    <t>Warehouse or other storage space, including, for instance, storage space for a strategic national stockpile or other stockpile of national  or international importance</t>
-  </si>
-  <si>
-    <t>Warehouses or storage facilities</t>
-  </si>
-  <si>
-    <t>Equipment for environmental monitoring, including including biological, chemical, or radiological remote sensing equipment that could be used for remote monitoring</t>
-  </si>
-  <si>
-    <t>Environmental monitoring equipment</t>
-  </si>
-  <si>
-    <t>Digital or computational resources required for data collection, analysis, or reporting, including infrastructure to collect survey data online or via phone</t>
-  </si>
-  <si>
-    <t>Data analysis and analytics infrastructure</t>
-  </si>
-  <si>
-    <t>Computing resources beyond those included as general overhead fees for workforce, including additional computers or laptops, web hosting or cloud computing resources, or tablets</t>
-  </si>
-  <si>
-    <t>Computing resources</t>
-  </si>
-  <si>
-    <t>Transportation resources and resources to ensure a secure cold chain, including packaging and supplies needed to ship materials and/or specimen referral systems</t>
-  </si>
-  <si>
-    <t>Transportation and transport fees, including cold chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water infrastructure and resources, including costs associated with water, sanitation, and hygiene (WASH) resources </t>
-  </si>
-  <si>
-    <t>Water resources and WASH</t>
-  </si>
-  <si>
-    <t>Fees associated with the printing and dissemination of information via print (e.g., newsletters, magazines, newspapers, printed documents, posters, peer-reviewed journals), radio, television, or online, or to host a national hotline</t>
-  </si>
-  <si>
-    <t>Subscriptions for various types of media including print (e.g., newsletters, magazines, newspapers), radio, or television</t>
-  </si>
-  <si>
-    <t>Media subscriptions</t>
-  </si>
-  <si>
-    <t>Select medical countermeasures, including vaccines, antivirals, antimicrobials, and other biologics, drugs, or devices that may be used in the event of a potential public health emergency</t>
-  </si>
-  <si>
-    <t>Medical countermeasures</t>
-  </si>
-  <si>
-    <t>Basic supplies for outbreak investigation and response, including supplies for vector control and sample collection and rapid response tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic supplies for outbreak investigation and response </t>
-  </si>
-  <si>
-    <t>Personal protective equipment, including supplies for biosafety incidents and emergency response</t>
-  </si>
-  <si>
-    <t>Personal protective equipment and basic supplies for infection prevention and control (IPC)</t>
-  </si>
-  <si>
-    <t>Added definitions for cost categories and subcategories</t>
-  </si>
-  <si>
-    <t>Adding documentation</t>
-  </si>
-  <si>
-    <t>Media distribution costs</t>
-  </si>
-  <si>
-    <t>The data dictionary was last updated on August 18, 2023</t>
-  </si>
-  <si>
-    <t>Revised select names and definitions of cost subcategories</t>
+Additional healthcare workers (doctors, nurses, and midwives)</t>
+    </r>
+  </si>
+  <si>
+    <t>global_health_emergency_corps_level</t>
+  </si>
+  <si>
+    <t>Global health emergency corps level</t>
+  </si>
+  <si>
+    <t>Connected health emergency leadership</t>
+  </si>
+  <si>
+    <t>Interoperable surge deployment</t>
+  </si>
+  <si>
+    <t>Health emergency corps</t>
+  </si>
+  <si>
+    <t>National public health and emergency workforce</t>
+  </si>
+  <si>
+    <t>Investments associated with predictiable and institutionalized coordination between senior-level strategic and technical health emergency leaders during preparedness and response</t>
+  </si>
+  <si>
+    <t>Investments associated with enhancing the quality, predictiability, and interoperability of national surge capacity by strengthening rapid response capacities and leveraging existing networks and mechanisms on the basis of common quality standards and coordination protocols (e.g., EMT, GOARN, GHC, SBPs, AVoHC/SURGE, etc.)</t>
+  </si>
+  <si>
+    <t>Specifies which, if any, administrative level of the WHO global health emergency corps architecture the line-item corresponds to. Note that not all line-items correspond to a level of the emergency corps. In cases where a single line-item could potentially align to more than one level of the architecture, the highest relevant level is specified.</t>
+  </si>
+  <si>
+    <t>Investments associated with implementing the WHO roadmap to increase national workforce capacity to deliver the essential public health functions (EPHFs), including a focus on emergency preparedness and response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definition from WHO: World Health Organization. Global Health Emergency Corps. 2023 Jul. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>One of:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Connected health emergency leadership
+Interoperable surge deployment
+Health emergency corps
+National public health and emergency workforce
+None</t>
+    </r>
+  </si>
+  <si>
+    <t>Investments associated with strengthening national workforce capacity of health emergency leaders, experts, and surge teams for alert, response and preparedness coordination and implementation (e.g., professionalization of occupations, where relevant)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1591,6 +1679,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1672,7 +1768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1788,6 +1884,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2029,8 +2131,8 @@
   </sheetPr>
   <dimension ref="A2:W1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2044,31 +2146,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
     </row>
     <row r="3" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="46" t="s">
         <v>451</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
     </row>
     <row r="4" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
     </row>
     <row r="5" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -2078,14 +2180,14 @@
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:23" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:23" s="12" customFormat="1" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -4357,17 +4459,17 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T999"/>
+  <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.19921875" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="35.3984375" customWidth="1"/>
+    <col min="3" max="3" width="38.796875" customWidth="1"/>
     <col min="4" max="4" width="67.3984375" customWidth="1"/>
     <col min="5" max="5" width="91.796875" customWidth="1"/>
   </cols>
@@ -4379,13 +4481,13 @@
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:20" s="18" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:20" s="19" customFormat="1" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
@@ -5399,7 +5501,7 @@
         <v>290</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E35" s="26"/>
       <c r="F35" s="28"/>
@@ -5429,7 +5531,7 @@
         <v>291</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E36" s="26"/>
       <c r="F36" s="28"/>
@@ -6058,7 +6160,7 @@
       </c>
       <c r="E60" s="30"/>
     </row>
-    <row r="61" spans="1:20" s="29" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" s="29" customFormat="1" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="29" t="s">
         <v>172</v>
       </c>
@@ -6069,27 +6171,27 @@
         <v>352</v>
       </c>
       <c r="D61" s="30" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" s="29" customFormat="1" ht="101" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="29" t="s">
         <v>172</v>
       </c>
       <c r="B62" s="29" t="s">
-        <v>334</v>
+        <v>454</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>353</v>
+        <v>455</v>
       </c>
       <c r="D62" s="30" t="s">
-        <v>369</v>
+        <v>462</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>379</v>
+        <v>465</v>
       </c>
     </row>
     <row r="63" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -6097,28 +6199,30 @@
         <v>172</v>
       </c>
       <c r="B63" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C63" s="29" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D63" s="30" t="s">
-        <v>370</v>
-      </c>
-      <c r="E63" s="30"/>
+        <v>369</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="64" spans="1:20" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="29" t="s">
         <v>172</v>
       </c>
       <c r="B64" s="29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E64" s="30"/>
     </row>
@@ -6127,13 +6231,13 @@
         <v>172</v>
       </c>
       <c r="B65" s="29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E65" s="30"/>
     </row>
@@ -6142,13 +6246,13 @@
         <v>172</v>
       </c>
       <c r="B66" s="29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D66" s="30" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E66" s="30"/>
     </row>
@@ -6157,13 +6261,13 @@
         <v>172</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E67" s="30"/>
     </row>
@@ -6172,13 +6276,13 @@
         <v>172</v>
       </c>
       <c r="B68" s="29" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D68" s="30" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E68" s="30"/>
     </row>
@@ -6187,17 +6291,31 @@
         <v>172</v>
       </c>
       <c r="B69" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="C69" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="D69" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="E69" s="30"/>
+    </row>
+    <row r="70" spans="1:5" s="29" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70" s="29" t="s">
         <v>341</v>
       </c>
-      <c r="C69" s="29" t="s">
+      <c r="C70" s="29" t="s">
         <v>360</v>
       </c>
-      <c r="D69" s="30" t="s">
+      <c r="D70" s="30" t="s">
         <v>374</v>
       </c>
-      <c r="E69" s="30"/>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="E70" s="30"/>
+    </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7127,6 +7245,7 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E2"/>
@@ -7144,17 +7263,17 @@
   </sheetPr>
   <dimension ref="A1:S1023"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" style="37" customWidth="1"/>
-    <col min="2" max="2" width="27.19921875" style="37" customWidth="1"/>
-    <col min="3" max="3" width="31.59765625" style="37" customWidth="1"/>
-    <col min="4" max="4" width="66.19921875" style="37" customWidth="1"/>
-    <col min="5" max="5" width="93" style="37" customWidth="1"/>
+    <col min="2" max="2" width="49" style="37" customWidth="1"/>
+    <col min="3" max="3" width="31.59765625" style="45" customWidth="1"/>
+    <col min="4" max="4" width="127.59765625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="80.19921875" style="37" customWidth="1"/>
     <col min="6" max="16384" width="14.3984375" style="37"/>
   </cols>
   <sheetData>
@@ -7163,13 +7282,13 @@
       <c r="B1" s="36"/>
     </row>
     <row r="2" spans="1:19" s="38" customFormat="1" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" spans="1:19" ht="29" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
@@ -7289,10 +7408,10 @@
         <v>279</v>
       </c>
       <c r="C7" s="34" t="s">
+        <v>400</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>401</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>402</v>
       </c>
       <c r="E7" s="34"/>
       <c r="F7" s="35"/>
@@ -7318,10 +7437,10 @@
         <v>279</v>
       </c>
       <c r="C8" s="34" t="s">
+        <v>402</v>
+      </c>
+      <c r="D8" s="34" t="s">
         <v>403</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>404</v>
       </c>
       <c r="E8" s="34"/>
       <c r="F8" s="35"/>
@@ -7347,10 +7466,10 @@
         <v>279</v>
       </c>
       <c r="C9" s="34" t="s">
+        <v>404</v>
+      </c>
+      <c r="D9" s="34" t="s">
         <v>405</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>406</v>
       </c>
       <c r="E9" s="34"/>
       <c r="F9" s="35"/>
@@ -7376,10 +7495,10 @@
         <v>279</v>
       </c>
       <c r="C10" s="34" t="s">
+        <v>406</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>407</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>408</v>
       </c>
       <c r="E10" s="34"/>
       <c r="F10" s="35"/>
@@ -7405,13 +7524,13 @@
         <v>279</v>
       </c>
       <c r="C11" s="34" t="s">
+        <v>408</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>411</v>
+      </c>
+      <c r="E11" s="34" t="s">
         <v>409</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>412</v>
-      </c>
-      <c r="E11" s="34" t="s">
-        <v>410</v>
       </c>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
@@ -7436,10 +7555,10 @@
         <v>279</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E12" s="34"/>
       <c r="F12" s="35"/>
@@ -7465,10 +7584,10 @@
         <v>280</v>
       </c>
       <c r="C13" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="D13" s="34" t="s">
         <v>415</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>416</v>
       </c>
       <c r="E13" s="34"/>
       <c r="F13" s="35"/>
@@ -7494,10 +7613,10 @@
         <v>280</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E14" s="34"/>
       <c r="F14" s="35"/>
@@ -7523,10 +7642,10 @@
         <v>280</v>
       </c>
       <c r="C15" s="34" t="s">
+        <v>418</v>
+      </c>
+      <c r="D15" s="34" t="s">
         <v>419</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>420</v>
       </c>
       <c r="E15" s="34"/>
       <c r="F15" s="35"/>
@@ -7552,10 +7671,10 @@
         <v>280</v>
       </c>
       <c r="C16" s="34" t="s">
+        <v>420</v>
+      </c>
+      <c r="D16" s="34" t="s">
         <v>421</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>422</v>
       </c>
       <c r="E16" s="34"/>
       <c r="F16" s="35"/>
@@ -7581,10 +7700,10 @@
         <v>280</v>
       </c>
       <c r="C17" s="34" t="s">
+        <v>422</v>
+      </c>
+      <c r="D17" s="34" t="s">
         <v>423</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>424</v>
       </c>
       <c r="E17" s="34"/>
       <c r="F17" s="35"/>
@@ -7610,10 +7729,10 @@
         <v>280</v>
       </c>
       <c r="C18" s="34" t="s">
+        <v>424</v>
+      </c>
+      <c r="D18" s="34" t="s">
         <v>425</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>426</v>
       </c>
       <c r="E18" s="34"/>
       <c r="F18" s="35"/>
@@ -7639,10 +7758,10 @@
         <v>280</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E19" s="34"/>
       <c r="F19" s="35"/>
@@ -7668,10 +7787,10 @@
         <v>280</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E20" s="34"/>
       <c r="F20" s="35"/>
@@ -7697,10 +7816,10 @@
         <v>280</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E21" s="34"/>
       <c r="F21" s="35"/>
@@ -7726,10 +7845,10 @@
         <v>280</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E22" s="34"/>
       <c r="F22" s="35"/>
@@ -7755,10 +7874,10 @@
         <v>280</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E23" s="34"/>
       <c r="F23" s="35"/>
@@ -7784,10 +7903,10 @@
         <v>280</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E24" s="34"/>
       <c r="F24" s="35"/>
@@ -7813,10 +7932,10 @@
         <v>280</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E25" s="34"/>
       <c r="F25" s="35"/>
@@ -7842,10 +7961,10 @@
         <v>280</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E26" s="34"/>
       <c r="F26" s="35"/>
@@ -7871,10 +7990,10 @@
         <v>280</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E27" s="34"/>
       <c r="F27" s="35"/>
@@ -7900,10 +8019,10 @@
         <v>280</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D28" s="34" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E28" s="34"/>
       <c r="F28" s="35"/>
@@ -7929,10 +8048,10 @@
         <v>280</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E29" s="34"/>
       <c r="F29" s="35"/>
@@ -7964,7 +8083,7 @@
         <v>383</v>
       </c>
       <c r="E30" s="34" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F30" s="35"/>
       <c r="G30" s="35"/>
@@ -7989,10 +8108,10 @@
         <v>333</v>
       </c>
       <c r="C31" s="34" t="s">
+        <v>393</v>
+      </c>
+      <c r="D31" s="34" t="s">
         <v>394</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>395</v>
       </c>
       <c r="E31" s="35"/>
       <c r="F31" s="35"/>
@@ -8134,13 +8253,13 @@
         <v>333</v>
       </c>
       <c r="C36" s="34" t="s">
+        <v>396</v>
+      </c>
+      <c r="D36" s="34" t="s">
         <v>397</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="E36" s="34" t="s">
         <v>398</v>
-      </c>
-      <c r="E36" s="34" t="s">
-        <v>399</v>
       </c>
       <c r="F36" s="42"/>
       <c r="G36" s="42"/>
@@ -8158,11 +8277,21 @@
       <c r="S36" s="42"/>
     </row>
     <row r="37" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="42"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
+      <c r="A37" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>456</v>
+      </c>
+      <c r="D37" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>464</v>
+      </c>
       <c r="F37" s="42"/>
       <c r="G37" s="42"/>
       <c r="H37" s="42"/>
@@ -8179,11 +8308,21 @@
       <c r="S37" s="42"/>
     </row>
     <row r="38" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="42"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
+      <c r="A38" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>457</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>464</v>
+      </c>
       <c r="F38" s="42"/>
       <c r="G38" s="42"/>
       <c r="H38" s="42"/>
@@ -8200,11 +8339,21 @@
       <c r="S38" s="42"/>
     </row>
     <row r="39" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="42"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
+      <c r="A39" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>458</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>466</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>464</v>
+      </c>
       <c r="F39" s="42"/>
       <c r="G39" s="42"/>
       <c r="H39" s="42"/>
@@ -8221,11 +8370,21 @@
       <c r="S39" s="42"/>
     </row>
     <row r="40" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="42"/>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
+      <c r="A40" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>464</v>
+      </c>
       <c r="F40" s="42"/>
       <c r="G40" s="42"/>
       <c r="H40" s="42"/>
@@ -9001,949 +9160,949 @@
     <row r="78" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="79" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="80" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1001" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1002" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1003" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1004" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1005" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1006" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1007" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1008" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1009" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1010" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1011" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1012" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1013" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1014" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1015" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1016" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1017" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1018" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1019" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1020" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1021" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1022" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1023" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:E2"/>
@@ -9979,13 +10138,13 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:19" s="18" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:19" s="20" customFormat="1" ht="25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
@@ -10040,10 +10199,10 @@
         <v>45135</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>448</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>449</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>381</v>
@@ -10071,10 +10230,10 @@
         <v>45156</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>381</v>
@@ -10098,11 +10257,21 @@
       <c r="S6" s="2"/>
     </row>
     <row r="7" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="A7" s="44">
+        <v>45226</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>155</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>

</xml_diff>